<commit_message>
ci: add new forms
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Ivory Coast/2023/ci_lf_pretas_2_participant_202302.xlsx
+++ b/LF/PreTAS/Ivory Coast/2023/ci_lf_pretas_2_participant_202302.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jboulinzann\Documents\Mes dev\WHO\FORMS\Côte d'Ivoire\Ivory Coast\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\WHO\dsa-forms\LF\PreTAS\Ivory Coast\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9F30F9-689C-465C-ACAD-37F8C9777E96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FDDF51-8760-4C90-95F8-6CBD5D417E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="138">
   <si>
     <t>form_title</t>
   </si>
@@ -38,9 +38,6 @@
     <t>form_id</t>
   </si>
   <si>
-    <t>version</t>
-  </si>
-  <si>
     <t>list_name</t>
   </si>
   <si>
@@ -365,10 +362,88 @@
     <t>Numéro d'ordre</t>
   </si>
   <si>
-    <t>(April 2022) 2. Côte d'Ivoire -  Pre TAS FL Formulaire Participants V1</t>
-  </si>
-  <si>
-    <t>ci_lf_pretas_2_participant_202204_v1</t>
+    <t>ci_lf_pretas_2_participant_202302</t>
+  </si>
+  <si>
+    <t>(2023 Fév) 2. Côte d'Ivoire -  Pre TAS FL Formulaire Participants V1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jamais </t>
+  </si>
+  <si>
+    <t xml:space="preserve">une fois </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 fois ou plus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Never </t>
+  </si>
+  <si>
+    <t xml:space="preserve">once </t>
+  </si>
+  <si>
+    <t>2 or more times</t>
+  </si>
+  <si>
+    <t>times</t>
+  </si>
+  <si>
+    <t>select_one times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combien de fois avez-vous pris des médicaments contre la FL </t>
+  </si>
+  <si>
+    <t>How often have you taken LF medication?</t>
+  </si>
+  <si>
+    <t>Absent pendant le TDM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peur des effets secondaires </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je n'étais pas au courant du TDM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le distributeur n'est pas venu chez moi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autres raisons </t>
+  </si>
+  <si>
+    <t>Absent during CT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fear of side effects </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I didn't know about the CT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The distributor did not come to my house </t>
+  </si>
+  <si>
+    <t>Other reasons</t>
+  </si>
+  <si>
+    <t>reasons</t>
+  </si>
+  <si>
+    <t>select_one reasons</t>
+  </si>
+  <si>
+    <t>p_took_med</t>
+  </si>
+  <si>
+    <t>p_reason_med</t>
+  </si>
+  <si>
+    <t>Jamais</t>
+  </si>
+  <si>
+    <t>${p_consent} = 'Yes' and ${p_took_med} = 'Jamais'</t>
   </si>
 </sst>
 </file>
@@ -500,7 +575,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -511,14 +586,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -530,22 +602,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -828,530 +896,593 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L14" sqref="L14"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18:XFD24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.19921875" customWidth="1"/>
+    <col min="3" max="3" width="42.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.25" customWidth="1"/>
     <col min="5" max="5" width="47.5" customWidth="1"/>
-    <col min="6" max="6" width="47.3984375" customWidth="1"/>
-    <col min="7" max="7" width="12.59765625" customWidth="1"/>
-    <col min="8" max="8" width="16.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.375" customWidth="1"/>
+    <col min="7" max="7" width="12.625" customWidth="1"/>
+    <col min="8" max="8" width="16.875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29.5" customWidth="1"/>
-    <col min="11" max="11" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="84.69921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.69921875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.3984375" customWidth="1"/>
-    <col min="15" max="15" width="13.8984375" customWidth="1"/>
-    <col min="16" max="16" width="36.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="84.75" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.375" customWidth="1"/>
+    <col min="15" max="15" width="13.875" customWidth="1"/>
+    <col min="16" max="16" width="36.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="12" t="s">
+      <c r="H1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="12" t="s">
+      <c r="J1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="12" t="s">
+      <c r="F2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+    </row>
+    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-    </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="B3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
       <c r="M3" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-    </row>
-    <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+    </row>
+    <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
-      <c r="P4" s="7"/>
-    </row>
-    <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="3"/>
       <c r="M5" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
-      <c r="P5" s="7"/>
-    </row>
-    <row r="6" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
-      <c r="P6" s="7"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" t="s">
+        <v>94</v>
+      </c>
+      <c r="K7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" t="s">
         <v>95</v>
       </c>
-      <c r="K7" t="s">
-        <v>99</v>
-      </c>
-      <c r="M7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="K8" t="s">
         <v>98</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="7"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="1:17" s="1" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="D10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3"/>
+      <c r="H10" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="7" t="s">
+      <c r="I10" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>109</v>
-      </c>
       <c r="K10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L10" s="3"/>
       <c r="M10" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
     </row>
-    <row r="11" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="4"/>
       <c r="I11" s="3"/>
       <c r="K11" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
     </row>
-    <row r="12" spans="1:17" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="10" t="s">
+    <row r="12" spans="1:17" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="J12" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="J12" s="4" t="s">
-        <v>66</v>
-      </c>
       <c r="K12" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
     </row>
-    <row r="13" spans="1:17" s="1" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F13" s="3"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="7" t="s">
+      <c r="G13" s="7"/>
+      <c r="H13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="L13" s="7"/>
+      <c r="M13" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J13" s="3" t="s">
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+    </row>
+    <row r="14" spans="1:17" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="K14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="M15" s="4"/>
+    </row>
+    <row r="16" spans="1:17" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L16" s="3"/>
+      <c r="M16" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+    </row>
+    <row r="17" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L17" s="3"/>
+      <c r="M17" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+    </row>
+    <row r="18" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="B18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="K18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="L13" s="8"/>
-      <c r="M13" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-    </row>
-    <row r="14" spans="1:17" s="1" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="F14" s="11"/>
-      <c r="K14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" s="1" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="11" t="s">
+      <c r="M18" s="4"/>
+    </row>
+    <row r="19" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11" t="s">
+      <c r="C19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="K15" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="M15" s="4"/>
-    </row>
-    <row r="16" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="B20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="B21" t="s">
         <v>36</v>
-      </c>
-      <c r="B18" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1362,92 +1493,204 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>4</v>
-      </c>
       <c r="C1" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
         <v>61</v>
       </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" t="s">
-        <v>62</v>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C13" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1455,26 +1698,26 @@
     <sortCondition ref="B9:B54"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1482,24 +1725,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2">
-        <v>20220405</v>
-      </c>
-      <c r="D2" t="s">
-        <v>79</v>
+        <v>110</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>